<commit_message>
Fix excel date parsing
</commit_message>
<xml_diff>
--- a/agenda-generator/samples/example-planning.xlsx
+++ b/agenda-generator/samples/example-planning.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_clones\agenda-generator\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_clones\hr-buddy\agenda-generator\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9450" yWindow="3240" windowWidth="12330" windowHeight="6060"/>
+    <workbookView xWindow="9450" yWindow="3240" windowWidth="12330" windowHeight="6060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="6" r:id="rId1"/>
@@ -1052,7 +1052,7 @@
   </sheetPr>
   <dimension ref="A2:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
@@ -1724,7 +1724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1740,7 +1740,7 @@
         <v>50</v>
       </c>
       <c r="B1" s="35">
-        <v>25570</v>
+        <v>43228</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>